<commit_message>
A whole bunch of edits and code cleanup.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/DRI_IOM_V8.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/DRI_IOM_V8.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/nutmod/data-raw/NutrientData/nutrientDetails/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BD01A9-14D0-2344-9960-883F8986A538}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43340" yWindow="-1400" windowWidth="22640" windowHeight="14600" activeTab="7"/>
+    <workbookView xWindow="9740" yWindow="460" windowWidth="22640" windowHeight="14600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="10" r:id="rId1"/>
@@ -25,7 +26,7 @@
     <sheet name="PR_zinc" sheetId="16" r:id="rId11"/>
     <sheet name="PR_iron" sheetId="17" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="108">
   <si>
     <t>Children</t>
   </si>
@@ -367,7 +368,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -528,77 +529,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -890,7 +826,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -994,7 +930,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1002,7 +938,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2373,7 +2309,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2710,7 +2646,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3055,7 +2991,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4839,7 +4775,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6081,7 +6017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7394,7 +7330,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8082,11 +8018,587 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:R1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="1">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>60</v>
+      </c>
+      <c r="H2" s="1">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="1">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F3" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="1">
+        <v>95</v>
+      </c>
+      <c r="H3" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="2">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G4" s="2">
+        <v>45</v>
+      </c>
+      <c r="H4" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="2">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G5" s="2">
+        <v>45</v>
+      </c>
+      <c r="H5" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="2">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G6" s="2">
+        <v>45</v>
+      </c>
+      <c r="H6" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="2">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G7" s="2">
+        <v>45</v>
+      </c>
+      <c r="H7" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="2">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G8" s="2">
+        <v>45</v>
+      </c>
+      <c r="H8" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="2">
+        <v>20</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G9" s="2">
+        <v>45</v>
+      </c>
+      <c r="H9" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="2">
+        <v>20</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G10" s="2">
+        <v>45</v>
+      </c>
+      <c r="H10" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="2">
+        <v>20</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G11" s="2">
+        <v>45</v>
+      </c>
+      <c r="H11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="2">
+        <v>25</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G12" s="2">
+        <v>45</v>
+      </c>
+      <c r="H12" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="2">
+        <v>25</v>
+      </c>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G13" s="2">
+        <v>45</v>
+      </c>
+      <c r="H13" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="2">
+        <v>20</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G14" s="2">
+        <v>45</v>
+      </c>
+      <c r="H14" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="2">
+        <v>20</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G15" s="2">
+        <v>45</v>
+      </c>
+      <c r="H15" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="2">
+        <v>20</v>
+      </c>
+      <c r="E16" s="2">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G16" s="2">
+        <v>45</v>
+      </c>
+      <c r="H16" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="2">
+        <v>20</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G17" s="2">
+        <v>45</v>
+      </c>
+      <c r="H17" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="2">
+        <v>20</v>
+      </c>
+      <c r="E18" s="2">
+        <v>5</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G18" s="2">
+        <v>45</v>
+      </c>
+      <c r="H18" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="2">
+        <v>20</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G19" s="2">
+        <v>45</v>
+      </c>
+      <c r="H19" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="2">
+        <v>20</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G20" s="2">
+        <v>45</v>
+      </c>
+      <c r="H20" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="2">
+        <v>20</v>
+      </c>
+      <c r="E21" s="2">
+        <v>5</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G21" s="2">
+        <v>45</v>
+      </c>
+      <c r="H21" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="2">
+        <v>20</v>
+      </c>
+      <c r="E22" s="2">
+        <v>5</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G22" s="2">
+        <v>45</v>
+      </c>
+      <c r="H22" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="2">
+        <v>20</v>
+      </c>
+      <c r="E23" s="2">
+        <v>5</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G23" s="2">
+        <v>45</v>
+      </c>
+      <c r="H23" s="2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8136,7 +8648,7 @@
       <c r="D2" s="1">
         <v>31</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="17">
         <v>4.4000000000000004</v>
       </c>
       <c r="F2" s="17">
@@ -8145,7 +8657,7 @@
       <c r="G2" s="1">
         <v>60</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="17">
         <v>9.1</v>
       </c>
       <c r="J2" s="2"/>
@@ -8166,7 +8678,7 @@
       <c r="D3" s="1">
         <v>30</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="17">
         <v>4.5999999999999996</v>
       </c>
       <c r="F3" s="17">
@@ -8175,7 +8687,7 @@
       <c r="G3" s="1">
         <v>95</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="17">
         <v>11</v>
       </c>
       <c r="J3" s="2"/>
@@ -8188,19 +8700,19 @@
         <v>69</v>
       </c>
       <c r="D4" s="2">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G4" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G4" s="6">
+        <v>65</v>
       </c>
       <c r="H4" s="2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -8219,19 +8731,19 @@
         <v>70</v>
       </c>
       <c r="D5" s="2">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E5" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G5" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G5" s="6">
+        <v>65</v>
       </c>
       <c r="H5" s="2">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -8250,19 +8762,19 @@
         <v>86</v>
       </c>
       <c r="D6" s="2">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E6" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G6" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G6" s="6">
+        <v>65</v>
       </c>
       <c r="H6" s="2">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -8281,19 +8793,19 @@
         <v>71</v>
       </c>
       <c r="D7" s="2">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G7" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G7" s="6">
+        <v>65</v>
       </c>
       <c r="H7" s="2">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -8310,19 +8822,19 @@
         <v>72</v>
       </c>
       <c r="D8" s="2">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E8" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F8" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G8" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G8" s="6">
+        <v>65</v>
       </c>
       <c r="H8" s="2">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -8339,19 +8851,19 @@
         <v>73</v>
       </c>
       <c r="D9" s="2">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F9" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G9" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G9" s="6">
+        <v>65</v>
       </c>
       <c r="H9" s="2">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -8368,19 +8880,19 @@
         <v>87</v>
       </c>
       <c r="D10" s="2">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E10" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F10" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G10" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G10" s="6">
+        <v>65</v>
       </c>
       <c r="H10" s="2">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -8397,19 +8909,19 @@
         <v>74</v>
       </c>
       <c r="D11" s="2">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E11" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F11" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G11" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G11" s="6">
+        <v>65</v>
       </c>
       <c r="H11" s="2">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -8428,19 +8940,19 @@
         <v>88</v>
       </c>
       <c r="D12" s="2">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F12" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G12" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G12" s="6">
+        <v>65</v>
       </c>
       <c r="H12" s="2">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -8457,19 +8969,19 @@
         <v>75</v>
       </c>
       <c r="D13" s="2">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E13" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F13" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G13" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G13" s="6">
+        <v>65</v>
       </c>
       <c r="H13" s="2">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -8486,19 +8998,19 @@
         <v>76</v>
       </c>
       <c r="D14" s="2">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E14" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F14" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G14" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G14" s="6">
+        <v>65</v>
       </c>
       <c r="H14" s="2">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -8515,19 +9027,19 @@
         <v>77</v>
       </c>
       <c r="D15" s="2">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E15" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F15" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G15" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G15" s="6">
+        <v>65</v>
       </c>
       <c r="H15" s="2">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -8544,19 +9056,19 @@
         <v>89</v>
       </c>
       <c r="D16" s="2">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E16" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F16" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G16" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G16" s="6">
+        <v>65</v>
       </c>
       <c r="H16" s="2">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -8573,19 +9085,19 @@
         <v>78</v>
       </c>
       <c r="D17" s="2">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E17" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F17" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G17" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G17" s="6">
+        <v>65</v>
       </c>
       <c r="H17" s="2">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -8602,19 +9114,19 @@
         <v>79</v>
       </c>
       <c r="D18" s="2">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E18" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F18" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G18" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G18" s="6">
+        <v>65</v>
       </c>
       <c r="H18" s="2">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -8631,19 +9143,19 @@
         <v>80</v>
       </c>
       <c r="D19" s="2">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E19" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F19" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G19" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G19" s="6">
+        <v>65</v>
       </c>
       <c r="H19" s="2">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -8660,19 +9172,19 @@
         <v>81</v>
       </c>
       <c r="D20" s="2">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E20" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F20" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G20" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G20" s="6">
+        <v>65</v>
       </c>
       <c r="H20" s="2">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -8689,19 +9201,19 @@
         <v>82</v>
       </c>
       <c r="D21" s="2">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E21" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F21" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G21" s="2">
-        <v>45</v>
+        <v>1.2</v>
+      </c>
+      <c r="G21" s="6">
+        <v>65</v>
       </c>
       <c r="H21" s="2">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -8718,688 +9230,6 @@
         <v>83</v>
       </c>
       <c r="D22" s="2">
-        <v>20</v>
-      </c>
-      <c r="E22" s="2">
-        <v>5</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G22" s="2">
-        <v>45</v>
-      </c>
-      <c r="H22" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="2">
-        <v>20</v>
-      </c>
-      <c r="E23" s="2">
-        <v>5</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G23" s="2">
-        <v>45</v>
-      </c>
-      <c r="H23" s="2">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N23"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="1" customWidth="1"/>
-    <col min="3" max="8" width="8.83203125" style="1"/>
-    <col min="10" max="16384" width="8.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="1">
-        <v>31</v>
-      </c>
-      <c r="E2" s="17">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="F2" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="G2" s="1">
-        <v>60</v>
-      </c>
-      <c r="H2" s="17">
-        <v>9.1</v>
-      </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="1">
-        <v>30</v>
-      </c>
-      <c r="E3" s="17">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="F3" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="G3" s="1">
-        <v>95</v>
-      </c>
-      <c r="H3" s="17">
-        <v>11</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="2">
-        <v>40</v>
-      </c>
-      <c r="E4" s="2">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G4" s="6">
-        <v>65</v>
-      </c>
-      <c r="H4" s="2">
-        <v>20</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="2">
-        <v>35</v>
-      </c>
-      <c r="E5" s="2">
-        <v>10</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G5" s="6">
-        <v>65</v>
-      </c>
-      <c r="H5" s="2">
-        <v>30</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="2">
-        <v>35</v>
-      </c>
-      <c r="E6" s="2">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G6" s="6">
-        <v>65</v>
-      </c>
-      <c r="H6" s="2">
-        <v>30</v>
-      </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="2">
-        <v>35</v>
-      </c>
-      <c r="E7" s="2">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G7" s="6">
-        <v>65</v>
-      </c>
-      <c r="H7" s="2">
-        <v>30</v>
-      </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="2">
-        <v>35</v>
-      </c>
-      <c r="E8" s="2">
-        <v>10</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G8" s="6">
-        <v>65</v>
-      </c>
-      <c r="H8" s="2">
-        <v>35</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="2">
-        <v>35</v>
-      </c>
-      <c r="E9" s="2">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G9" s="6">
-        <v>65</v>
-      </c>
-      <c r="H9" s="2">
-        <v>35</v>
-      </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="2">
-        <v>35</v>
-      </c>
-      <c r="E10" s="2">
-        <v>10</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G10" s="6">
-        <v>65</v>
-      </c>
-      <c r="H10" s="2">
-        <v>35</v>
-      </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="2">
-        <v>35</v>
-      </c>
-      <c r="E11" s="2">
-        <v>10</v>
-      </c>
-      <c r="F11" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G11" s="6">
-        <v>65</v>
-      </c>
-      <c r="H11" s="2">
-        <v>35</v>
-      </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="2">
-        <v>35</v>
-      </c>
-      <c r="E12" s="2">
-        <v>10</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G12" s="6">
-        <v>65</v>
-      </c>
-      <c r="H12" s="2">
-        <v>30</v>
-      </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="2">
-        <v>35</v>
-      </c>
-      <c r="E13" s="2">
-        <v>10</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G13" s="6">
-        <v>65</v>
-      </c>
-      <c r="H13" s="2">
-        <v>30</v>
-      </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="2">
-        <v>35</v>
-      </c>
-      <c r="E14" s="2">
-        <v>10</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G14" s="6">
-        <v>65</v>
-      </c>
-      <c r="H14" s="2">
-        <v>35</v>
-      </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="2">
-        <v>35</v>
-      </c>
-      <c r="E15" s="2">
-        <v>10</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G15" s="6">
-        <v>65</v>
-      </c>
-      <c r="H15" s="2">
-        <v>35</v>
-      </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="2">
-        <v>35</v>
-      </c>
-      <c r="E16" s="2">
-        <v>10</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G16" s="6">
-        <v>65</v>
-      </c>
-      <c r="H16" s="2">
-        <v>35</v>
-      </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" s="2">
-        <v>35</v>
-      </c>
-      <c r="E17" s="2">
-        <v>10</v>
-      </c>
-      <c r="F17" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G17" s="6">
-        <v>65</v>
-      </c>
-      <c r="H17" s="2">
-        <v>35</v>
-      </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="2">
-        <v>35</v>
-      </c>
-      <c r="E18" s="2">
-        <v>10</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G18" s="6">
-        <v>65</v>
-      </c>
-      <c r="H18" s="2">
-        <v>35</v>
-      </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" s="2">
-        <v>35</v>
-      </c>
-      <c r="E19" s="2">
-        <v>10</v>
-      </c>
-      <c r="F19" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G19" s="6">
-        <v>65</v>
-      </c>
-      <c r="H19" s="2">
-        <v>35</v>
-      </c>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="2">
-        <v>35</v>
-      </c>
-      <c r="E20" s="2">
-        <v>10</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G20" s="6">
-        <v>65</v>
-      </c>
-      <c r="H20" s="2">
-        <v>35</v>
-      </c>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="2">
-        <v>35</v>
-      </c>
-      <c r="E21" s="2">
-        <v>10</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G21" s="6">
-        <v>65</v>
-      </c>
-      <c r="H21" s="2">
-        <v>35</v>
-      </c>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="2">
         <v>35</v>
       </c>
       <c r="E22" s="2">
@@ -9415,7 +9245,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -9445,10 +9275,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -9744,7 +9574,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Lots of cleanup across several files.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/DRI_IOM_V8.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/DRI_IOM_V8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/nutmod/data-raw/NutrientData/nutrientDetails/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BD01A9-14D0-2344-9960-883F8986A538}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7DF9BA-1C94-8A40-964F-1C8817F06E51}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9740" yWindow="460" windowWidth="22640" windowHeight="14600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9720" yWindow="460" windowWidth="22640" windowHeight="14600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="10" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="PR_zinc" sheetId="16" r:id="rId11"/>
     <sheet name="PR_iron" sheetId="17" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -440,7 +440,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -509,6 +509,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -6020,8 +6029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6116,7 +6125,7 @@
       <c r="H2" s="7">
         <v>110</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="27">
         <v>0.27</v>
       </c>
       <c r="J2" s="7">
@@ -6172,7 +6181,7 @@
       <c r="H3" s="7">
         <v>130</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="28">
         <v>11</v>
       </c>
       <c r="J3" s="7">
@@ -6228,7 +6237,7 @@
       <c r="H4" s="2">
         <v>90</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="29">
         <v>7</v>
       </c>
       <c r="J4" s="2">
@@ -6284,7 +6293,7 @@
       <c r="H5" s="2">
         <v>90</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="29">
         <v>10</v>
       </c>
       <c r="J5" s="2">
@@ -6340,7 +6349,7 @@
       <c r="H6" s="2">
         <v>120</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="29">
         <v>8</v>
       </c>
       <c r="J6" s="2">
@@ -6396,7 +6405,7 @@
       <c r="H7" s="2">
         <v>150</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="29">
         <v>11</v>
       </c>
       <c r="J7" s="2">
@@ -6452,7 +6461,7 @@
       <c r="H8" s="2">
         <v>150</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="29">
         <v>8</v>
       </c>
       <c r="J8" s="2">
@@ -6508,7 +6517,7 @@
       <c r="H9" s="2">
         <v>150</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="29">
         <v>8</v>
       </c>
       <c r="J9" s="2">
@@ -6564,7 +6573,7 @@
       <c r="H10" s="2">
         <v>150</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="29">
         <v>8</v>
       </c>
       <c r="J10" s="2">
@@ -6620,7 +6629,7 @@
       <c r="H11" s="2">
         <v>150</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="29">
         <v>8</v>
       </c>
       <c r="J11" s="2">
@@ -6676,7 +6685,7 @@
       <c r="H12" s="2">
         <v>120</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="29">
         <v>8</v>
       </c>
       <c r="J12" s="2">
@@ -6732,7 +6741,7 @@
       <c r="H13" s="2">
         <v>150</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="29">
         <v>15</v>
       </c>
       <c r="J13" s="2">
@@ -6788,7 +6797,7 @@
       <c r="H14" s="2">
         <v>150</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="29">
         <v>18</v>
       </c>
       <c r="J14" s="2">
@@ -6844,7 +6853,7 @@
       <c r="H15" s="2">
         <v>150</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="29">
         <v>18</v>
       </c>
       <c r="J15" s="2">
@@ -6900,7 +6909,7 @@
       <c r="H16" s="2">
         <v>150</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="29">
         <v>8</v>
       </c>
       <c r="J16" s="2">
@@ -6956,7 +6965,7 @@
       <c r="H17" s="2">
         <v>150</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="29">
         <v>8</v>
       </c>
       <c r="J17" s="2">
@@ -7012,7 +7021,7 @@
       <c r="H18" s="2">
         <v>220</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="29">
         <v>27</v>
       </c>
       <c r="J18" s="2">
@@ -7068,7 +7077,7 @@
       <c r="H19" s="2">
         <v>220</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="29">
         <v>27</v>
       </c>
       <c r="J19" s="2">
@@ -7124,7 +7133,7 @@
       <c r="H20" s="2">
         <v>220</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="29">
         <v>27</v>
       </c>
       <c r="J20" s="2">
@@ -7180,7 +7189,7 @@
       <c r="H21" s="2">
         <v>290</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="29">
         <v>10</v>
       </c>
       <c r="J21" s="2">
@@ -7236,7 +7245,7 @@
       <c r="H22" s="2">
         <v>290</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="29">
         <v>9</v>
       </c>
       <c r="J22" s="2">
@@ -7292,7 +7301,7 @@
       <c r="H23" s="2">
         <v>290</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="29">
         <v>9</v>
       </c>
       <c r="J23" s="2">
@@ -8021,7 +8030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:R1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>